<commit_message>
update graph and README
</commit_message>
<xml_diff>
--- a/data/data_spreadsheet/data.xlsx
+++ b/data/data_spreadsheet/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,36 @@
           <t>File Name</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Westgate Compiled,5589,04:10:51,16:25:00.txt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -445,6 +475,36 @@
           <t>Vehicle Type</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>truck</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pedestrian</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>motorbike</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>bicycle</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -452,6 +512,36 @@
           <t>Time Initial</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>16:25:50</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -459,6 +549,36 @@
           <t>Time Final</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>20:35:51</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -466,6 +586,36 @@
           <t>Time Total</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>4:10:01</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -473,6 +623,24 @@
           <t>Total Vehicles</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>5588</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3992</v>
+      </c>
+      <c r="D6" t="n">
+        <v>631</v>
+      </c>
+      <c r="E6" t="n">
+        <v>141</v>
+      </c>
+      <c r="F6" t="n">
+        <v>399</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -480,6 +648,24 @@
           <t>Vehicles from Left</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>3090</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D7" t="n">
+        <v>465</v>
+      </c>
+      <c r="E7" t="n">
+        <v>98</v>
+      </c>
+      <c r="F7" t="n">
+        <v>221</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -487,6 +673,24 @@
           <t>Vehicles from Right</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>2498</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D8" t="n">
+        <v>166</v>
+      </c>
+      <c r="E8" t="n">
+        <v>43</v>
+      </c>
+      <c r="F8" t="n">
+        <v>178</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -494,6 +698,24 @@
           <t>Total Hours</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>4.166944444444445</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.166944444444445</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4.166944444444445</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.166944444444445</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.166944444444445</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4.166944444444445</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -501,6 +723,24 @@
           <t>Vehicles per Hour</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>1341.030597960136</v>
+      </c>
+      <c r="C10" t="n">
+        <v>958.0161322578494</v>
+      </c>
+      <c r="D10" t="n">
+        <v>151.4299046730218</v>
+      </c>
+      <c r="E10" t="n">
+        <v>33.83774415038997</v>
+      </c>
+      <c r="F10" t="n">
+        <v>95.75361642557162</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5.039664022398506</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -508,6 +748,24 @@
           <t>Vehicles per Hour from Left</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>741.5505632957802</v>
+      </c>
+      <c r="C11" t="n">
+        <v>475.8882741150589</v>
+      </c>
+      <c r="D11" t="n">
+        <v>111.5925604959669</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23.51843210452636</v>
+      </c>
+      <c r="F11" t="n">
+        <v>53.03646423571762</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.839744017065529</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -515,6 +773,24 @@
           <t>Vehicles per Hour from Right</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>599.4800346643557</v>
+      </c>
+      <c r="C12" t="n">
+        <v>482.1278581427904</v>
+      </c>
+      <c r="D12" t="n">
+        <v>39.83734417705486</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10.31931204586361</v>
+      </c>
+      <c r="F12" t="n">
+        <v>42.717152189854</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.199920005332978</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -522,6 +798,36 @@
           <t>Morning Peak Start Time</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -529,6 +835,36 @@
           <t>Morning Peak End Time</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -536,6 +872,36 @@
           <t>Morning Peak Total Vehicles</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -543,6 +909,36 @@
           <t>Morning Peak Total Hours</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -550,6 +946,36 @@
           <t>Morning Peak Vehicles per Hour</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -557,6 +983,36 @@
           <t>Morning Peak Vehicles from Left</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -564,6 +1020,36 @@
           <t>Morning Peak Vehicles from Right</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -571,6 +1057,36 @@
           <t>Morning Peak VpH from Left</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -578,6 +1094,36 @@
           <t>Morning Peak VpH from Right</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -585,6 +1131,36 @@
           <t>Night Peak Start Time</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -592,6 +1168,36 @@
           <t>Night Peak End Time</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -599,6 +1205,36 @@
           <t>Night Peak Total Vehicles</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -606,6 +1242,36 @@
           <t>Night Peak Total Hours</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -613,6 +1279,36 @@
           <t>Night Peak Vehicles per Hour</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -620,6 +1316,36 @@
           <t>Night Peak Vehicles from Left</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -627,6 +1353,36 @@
           <t>Night Peak Vehicles from Right</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -634,11 +1390,71 @@
           <t>Night Peak Vph from Left</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
           <t>Night Peak Vph from Right</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>